<commit_message>
Summary of missing values
</commit_message>
<xml_diff>
--- a/Identify Important Variables and Document Missing Values, Variable Types, Key Values, and Patterns/data_organization_total.xlsx
+++ b/Identify Important Variables and Document Missing Values, Variable Types, Key Values, and Patterns/data_organization_total.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="829">
   <si>
     <t xml:space="preserve">Variable_name_original</t>
   </si>
@@ -411,6 +411,27 @@
   </si>
   <si>
     <t xml:space="preserve">440111 (1477)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">行政区划代码</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.82%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">441901 (3300)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120116 (1492)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440306 (1404)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">442001 (1351)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330109 (1116)</t>
   </si>
   <si>
     <t xml:space="preserve">qh</t>
@@ -3314,116 +3335,116 @@
         <v>133</v>
       </c>
       <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
         <v>134</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s">
         <v>135</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>136</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>137</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>138</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>139</v>
-      </c>
-      <c r="I19" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" t="s">
         <v>141</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>142</v>
       </c>
-      <c r="C20" t="s">
-        <v>115</v>
-      </c>
       <c r="D20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I20" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>146</v>
-      </c>
-      <c r="F21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I21" t="s">
-        <v>150</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" t="s">
         <v>151</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>152</v>
-      </c>
-      <c r="C22" t="s">
-        <v>153</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" t="s">
         <v>154</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>155</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>156</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>157</v>
-      </c>
-      <c r="I22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
         <v>159</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>160</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -3455,7 +3476,7 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
         <v>168</v>
@@ -3484,7 +3505,7 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
         <v>175</v>
@@ -3513,7 +3534,7 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
         <v>182</v>
@@ -3542,7 +3563,7 @@
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
         <v>189</v>
@@ -3571,7 +3592,7 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
         <v>196</v>
@@ -3600,7 +3621,7 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
         <v>203</v>
@@ -3626,117 +3647,117 @@
         <v>209</v>
       </c>
       <c r="C30" t="s">
-        <v>210</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" t="s">
         <v>211</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>212</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>213</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>214</v>
-      </c>
-      <c r="I30" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" t="s">
         <v>216</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>217</v>
-      </c>
-      <c r="C31" t="s">
-        <v>218</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F31" t="s">
         <v>219</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>220</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>221</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>222</v>
-      </c>
-      <c r="I31" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" t="s">
         <v>224</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>225</v>
-      </c>
-      <c r="C32" t="s">
-        <v>226</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F32" t="s">
         <v>227</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>228</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>229</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>230</v>
-      </c>
-      <c r="I32" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33" t="s">
         <v>232</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>233</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
         <v>234</v>
       </c>
-      <c r="D33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>235</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>236</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>237</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>238</v>
-      </c>
-      <c r="I33" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B34" t="s">
         <v>240</v>
@@ -3797,39 +3818,39 @@
         <v>254</v>
       </c>
       <c r="B36" t="s">
+        <v>254</v>
+      </c>
+      <c r="C36" t="s">
         <v>255</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" t="s">
         <v>256</v>
       </c>
-      <c r="D36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>257</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>258</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>259</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>260</v>
-      </c>
-      <c r="I36" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>261</v>
+      </c>
+      <c r="B37" t="s">
         <v>262</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>263</v>
-      </c>
-      <c r="C37" t="s">
-        <v>256</v>
       </c>
       <c r="D37" t="s">
         <v>107</v>
@@ -3858,171 +3879,171 @@
         <v>270</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>263</v>
       </c>
       <c r="D38" t="s">
         <v>107</v>
       </c>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
+      <c r="E38" t="s">
+        <v>271</v>
+      </c>
+      <c r="F38" t="s">
+        <v>272</v>
+      </c>
+      <c r="G38" t="s">
+        <v>273</v>
+      </c>
+      <c r="H38" t="s">
+        <v>274</v>
+      </c>
+      <c r="I38" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
         <v>107</v>
       </c>
-      <c r="E39" t="s">
-        <v>274</v>
-      </c>
-      <c r="F39" t="s">
-        <v>275</v>
-      </c>
-      <c r="G39" t="s">
-        <v>276</v>
-      </c>
-      <c r="H39" t="s">
-        <v>277</v>
-      </c>
-      <c r="I39" t="s">
-        <v>278</v>
-      </c>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>278</v>
+      </c>
+      <c r="B40" t="s">
         <v>279</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>280</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" t="s">
         <v>281</v>
       </c>
-      <c r="D40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>282</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>283</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>284</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>285</v>
-      </c>
-      <c r="I40" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>286</v>
+      </c>
+      <c r="B41" t="s">
         <v>287</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>288</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
         <v>289</v>
       </c>
-      <c r="D41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>290</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>291</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>292</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>293</v>
-      </c>
-      <c r="I41" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>294</v>
+      </c>
+      <c r="B42" t="s">
         <v>295</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>296</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" t="s">
         <v>297</v>
       </c>
-      <c r="D42" t="s">
-        <v>107</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>298</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>299</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>300</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>301</v>
-      </c>
-      <c r="I42" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" t="s">
         <v>303</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>304</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" t="s">
         <v>305</v>
       </c>
-      <c r="D43" t="s">
-        <v>107</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>306</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>307</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>308</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>309</v>
-      </c>
-      <c r="I43" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>310</v>
+      </c>
+      <c r="B44" t="s">
         <v>311</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>312</v>
-      </c>
-      <c r="C44" t="s">
-        <v>297</v>
       </c>
       <c r="D44" t="s">
         <v>107</v>
@@ -4051,7 +4072,7 @@
         <v>319</v>
       </c>
       <c r="C45" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D45" t="s">
         <v>107</v>
@@ -4080,7 +4101,7 @@
         <v>326</v>
       </c>
       <c r="C46" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D46" t="s">
         <v>107</v>
@@ -4109,7 +4130,7 @@
         <v>333</v>
       </c>
       <c r="C47" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D47" t="s">
         <v>107</v>
@@ -4138,7 +4159,7 @@
         <v>340</v>
       </c>
       <c r="C48" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D48" t="s">
         <v>107</v>
@@ -4167,7 +4188,7 @@
         <v>347</v>
       </c>
       <c r="C49" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D49" t="s">
         <v>107</v>
@@ -4196,7 +4217,7 @@
         <v>354</v>
       </c>
       <c r="C50" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D50" t="s">
         <v>107</v>
@@ -4225,7 +4246,7 @@
         <v>361</v>
       </c>
       <c r="C51" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D51" t="s">
         <v>107</v>
@@ -4254,7 +4275,7 @@
         <v>368</v>
       </c>
       <c r="C52" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D52" t="s">
         <v>107</v>
@@ -4283,7 +4304,7 @@
         <v>375</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D53" t="s">
         <v>107</v>
@@ -4312,7 +4333,7 @@
         <v>382</v>
       </c>
       <c r="C54" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D54" t="s">
         <v>107</v>
@@ -4341,7 +4362,7 @@
         <v>389</v>
       </c>
       <c r="C55" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D55" t="s">
         <v>107</v>
@@ -4370,7 +4391,7 @@
         <v>396</v>
       </c>
       <c r="C56" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D56" t="s">
         <v>107</v>
@@ -4399,7 +4420,7 @@
         <v>403</v>
       </c>
       <c r="C57" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D57" t="s">
         <v>107</v>
@@ -4428,7 +4449,7 @@
         <v>410</v>
       </c>
       <c r="C58" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D58" t="s">
         <v>107</v>
@@ -4457,7 +4478,7 @@
         <v>417</v>
       </c>
       <c r="C59" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D59" t="s">
         <v>107</v>
@@ -4486,7 +4507,7 @@
         <v>424</v>
       </c>
       <c r="C60" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D60" t="s">
         <v>107</v>
@@ -4515,7 +4536,7 @@
         <v>431</v>
       </c>
       <c r="C61" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D61" t="s">
         <v>107</v>
@@ -4544,7 +4565,7 @@
         <v>438</v>
       </c>
       <c r="C62" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D62" t="s">
         <v>107</v>
@@ -4573,7 +4594,7 @@
         <v>445</v>
       </c>
       <c r="C63" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D63" t="s">
         <v>107</v>
@@ -4602,7 +4623,7 @@
         <v>452</v>
       </c>
       <c r="C64" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D64" t="s">
         <v>107</v>
@@ -4631,7 +4652,7 @@
         <v>459</v>
       </c>
       <c r="C65" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D65" t="s">
         <v>107</v>
@@ -4660,7 +4681,7 @@
         <v>466</v>
       </c>
       <c r="C66" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D66" t="s">
         <v>107</v>
@@ -4689,7 +4710,7 @@
         <v>473</v>
       </c>
       <c r="C67" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D67" t="s">
         <v>107</v>
@@ -4715,10 +4736,10 @@
         <v>479</v>
       </c>
       <c r="B68" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C68" t="s">
-        <v>480</v>
+        <v>304</v>
       </c>
       <c r="D68" t="s">
         <v>107</v>
@@ -4805,45 +4826,45 @@
         <v>500</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>501</v>
       </c>
       <c r="D71" t="s">
         <v>107</v>
       </c>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
+      <c r="E71" t="s">
+        <v>502</v>
+      </c>
+      <c r="F71" t="s">
+        <v>503</v>
+      </c>
+      <c r="G71" t="s">
+        <v>504</v>
+      </c>
+      <c r="H71" t="s">
+        <v>505</v>
+      </c>
+      <c r="I71" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="B72" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="C72" t="s">
-        <v>502</v>
+        <v>115</v>
       </c>
       <c r="D72" t="s">
         <v>107</v>
       </c>
-      <c r="E72" t="s">
-        <v>503</v>
-      </c>
-      <c r="F72" t="s">
-        <v>504</v>
-      </c>
-      <c r="G72" t="s">
-        <v>505</v>
-      </c>
-      <c r="H72" t="s">
-        <v>506</v>
-      </c>
-      <c r="I72" t="s">
-        <v>507</v>
-      </c>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
@@ -4998,45 +5019,45 @@
         <v>543</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>544</v>
       </c>
       <c r="D78" t="s">
         <v>107</v>
       </c>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
+      <c r="E78" t="s">
+        <v>545</v>
+      </c>
+      <c r="F78" t="s">
+        <v>546</v>
+      </c>
+      <c r="G78" t="s">
+        <v>547</v>
+      </c>
+      <c r="H78" t="s">
+        <v>548</v>
+      </c>
+      <c r="I78" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="B79" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="C79" t="s">
-        <v>545</v>
+        <v>115</v>
       </c>
       <c r="D79" t="s">
         <v>107</v>
       </c>
-      <c r="E79" t="s">
-        <v>546</v>
-      </c>
-      <c r="F79" t="s">
-        <v>547</v>
-      </c>
-      <c r="G79" t="s">
-        <v>548</v>
-      </c>
-      <c r="H79" t="s">
-        <v>549</v>
-      </c>
-      <c r="I79" t="s">
-        <v>550</v>
-      </c>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
@@ -5049,7 +5070,7 @@
         <v>552</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E80" t="s">
         <v>553</v>
@@ -5078,7 +5099,7 @@
         <v>559</v>
       </c>
       <c r="D81" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
         <v>560</v>
@@ -5281,7 +5302,7 @@
         <v>608</v>
       </c>
       <c r="D88" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E88" t="s">
         <v>609</v>
@@ -5310,7 +5331,7 @@
         <v>615</v>
       </c>
       <c r="D89" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="E89" t="s">
         <v>616</v>
@@ -5681,329 +5702,329 @@
         <v>705</v>
       </c>
       <c r="B102" t="s">
+        <v>705</v>
+      </c>
+      <c r="C102" t="s">
         <v>706</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>107</v>
+      </c>
+      <c r="E102" t="s">
         <v>707</v>
       </c>
-      <c r="D102" t="s">
-        <v>107</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>708</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
         <v>709</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>710</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
         <v>711</v>
-      </c>
-      <c r="I102" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>712</v>
+      </c>
+      <c r="B103" t="s">
         <v>713</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>714</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
+        <v>107</v>
+      </c>
+      <c r="E103" t="s">
         <v>715</v>
       </c>
-      <c r="D103" t="s">
-        <v>107</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>716</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G103" t="s">
         <v>717</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>718</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>719</v>
-      </c>
-      <c r="I103" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>720</v>
+      </c>
+      <c r="B104" t="s">
         <v>721</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>722</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" t="s">
         <v>723</v>
       </c>
-      <c r="D104" t="s">
-        <v>107</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>724</v>
       </c>
-      <c r="F104" t="s">
+      <c r="G104" t="s">
         <v>725</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" t="s">
         <v>726</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>727</v>
-      </c>
-      <c r="I104" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
+        <v>728</v>
+      </c>
+      <c r="B105" t="s">
         <v>729</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>730</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
+        <v>107</v>
+      </c>
+      <c r="E105" t="s">
         <v>731</v>
       </c>
-      <c r="D105" t="s">
-        <v>107</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>732</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
         <v>733</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>734</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>735</v>
-      </c>
-      <c r="I105" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
+        <v>736</v>
+      </c>
+      <c r="B106" t="s">
         <v>737</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>738</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>107</v>
+      </c>
+      <c r="E106" t="s">
         <v>739</v>
       </c>
-      <c r="D106" t="s">
-        <v>107</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>740</v>
       </c>
-      <c r="F106" t="s">
+      <c r="G106" t="s">
         <v>741</v>
       </c>
-      <c r="G106" t="s">
+      <c r="H106" t="s">
         <v>742</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>743</v>
-      </c>
-      <c r="I106" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
+        <v>744</v>
+      </c>
+      <c r="B107" t="s">
         <v>745</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>746</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
+        <v>107</v>
+      </c>
+      <c r="E107" t="s">
         <v>747</v>
       </c>
-      <c r="D107" t="s">
-        <v>107</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>748</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>749</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>750</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>751</v>
-      </c>
-      <c r="I107" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
+        <v>752</v>
+      </c>
+      <c r="B108" t="s">
         <v>753</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>754</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>107</v>
+      </c>
+      <c r="E108" t="s">
         <v>755</v>
       </c>
-      <c r="D108" t="s">
-        <v>107</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>756</v>
       </c>
-      <c r="F108" t="s">
+      <c r="G108" t="s">
         <v>757</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>758</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>759</v>
-      </c>
-      <c r="I108" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
+        <v>760</v>
+      </c>
+      <c r="B109" t="s">
         <v>761</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>762</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
+        <v>107</v>
+      </c>
+      <c r="E109" t="s">
         <v>763</v>
       </c>
-      <c r="D109" t="s">
-        <v>107</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>764</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>765</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>766</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>767</v>
-      </c>
-      <c r="I109" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
+        <v>768</v>
+      </c>
+      <c r="B110" t="s">
         <v>769</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>770</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" t="s">
         <v>771</v>
       </c>
-      <c r="D110" t="s">
-        <v>107</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>772</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
         <v>773</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>774</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>775</v>
-      </c>
-      <c r="I110" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>776</v>
+      </c>
+      <c r="B111" t="s">
         <v>777</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>778</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
+        <v>107</v>
+      </c>
+      <c r="E111" t="s">
         <v>779</v>
       </c>
-      <c r="D111" t="s">
-        <v>107</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>780</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>781</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>782</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>783</v>
-      </c>
-      <c r="I111" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>784</v>
+      </c>
+      <c r="B112" t="s">
         <v>785</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>786</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
+        <v>107</v>
+      </c>
+      <c r="E112" t="s">
         <v>787</v>
       </c>
-      <c r="D112" t="s">
-        <v>107</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>788</v>
       </c>
-      <c r="F112" t="s">
+      <c r="G112" t="s">
         <v>789</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>790</v>
       </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>791</v>
-      </c>
-      <c r="I112" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
+        <v>792</v>
+      </c>
+      <c r="B113" t="s">
         <v>793</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>794</v>
-      </c>
-      <c r="C113" t="s">
-        <v>787</v>
       </c>
       <c r="D113" t="s">
         <v>107</v>
@@ -6032,36 +6053,36 @@
         <v>801</v>
       </c>
       <c r="C114" t="s">
+        <v>794</v>
+      </c>
+      <c r="D114" t="s">
+        <v>107</v>
+      </c>
+      <c r="E114" t="s">
         <v>802</v>
       </c>
-      <c r="D114" t="s">
-        <v>107</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>803</v>
       </c>
-      <c r="F114" t="s">
+      <c r="G114" t="s">
         <v>804</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>805</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>806</v>
-      </c>
-      <c r="I114" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
+        <v>807</v>
+      </c>
+      <c r="B115" t="s">
         <v>808</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>809</v>
-      </c>
-      <c r="C115" t="s">
-        <v>802</v>
       </c>
       <c r="D115" t="s">
         <v>107</v>
@@ -6090,7 +6111,7 @@
         <v>816</v>
       </c>
       <c r="C116" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="D116" t="s">
         <v>107</v>
@@ -6109,6 +6130,35 @@
       </c>
       <c r="I116" t="s">
         <v>821</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>822</v>
+      </c>
+      <c r="B117" t="s">
+        <v>823</v>
+      </c>
+      <c r="C117" t="s">
+        <v>809</v>
+      </c>
+      <c r="D117" t="s">
+        <v>107</v>
+      </c>
+      <c r="E117" t="s">
+        <v>824</v>
+      </c>
+      <c r="F117" t="s">
+        <v>825</v>
+      </c>
+      <c r="G117" t="s">
+        <v>826</v>
+      </c>
+      <c r="H117" t="s">
+        <v>827</v>
+      </c>
+      <c r="I117" t="s">
+        <v>828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>